<commit_message>
item 7 power bi
</commit_message>
<xml_diff>
--- a/003-importacaoETratamentoDeBaseDeDadosComPowerQuery/Cadastro Produtos.xlsx
+++ b/003-importacaoETratamentoDeBaseDeDadosComPowerQuery/Cadastro Produtos.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e775ab26b5c1cdcb/Hashtag/Aulas Power BI/Power BI Impressionador/Módulo Power Query (Novo) - Backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\hashtag\hashtagPowerBI\003-importacaoETratamentoDeBaseDeDadosComPowerQuery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_FC6AF3798B78658470985F5E5199B4BA1B234724" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF42EA2B-46FC-4D65-8A92-912443A71C99}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE893A2-6827-44BB-AE24-CBBEA79F2936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Produtos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Produtos!$A$1:$D$25</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -455,20 +455,20 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,18 +755,18 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -789,7 +789,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -810,7 +810,7 @@
       </c>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
@@ -831,7 +831,7 @@
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
@@ -852,7 +852,7 @@
       </c>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -875,7 +875,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -896,7 +896,7 @@
       </c>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
@@ -917,7 +917,7 @@
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -938,7 +938,7 @@
       </c>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
@@ -959,7 +959,7 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -980,7 +980,7 @@
       </c>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>31</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>33</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>35</v>
       </c>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>39</v>
       </c>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="G22" s="13"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>41</v>
       </c>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
08 possiveis problemas no power query parte2 fim
</commit_message>
<xml_diff>
--- a/003-importacaoETratamentoDeBaseDeDadosComPowerQuery/Cadastro Produtos.xlsx
+++ b/003-importacaoETratamentoDeBaseDeDadosComPowerQuery/Cadastro Produtos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\hashtag\hashtagPowerBI\003-importacaoETratamentoDeBaseDeDadosComPowerQuery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jharbes\Documents\GitHub\hashtagPowerBI\003-importacaoETratamentoDeBaseDeDadosComPowerQuery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE893A2-6827-44BB-AE24-CBBEA79F2936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE03936-2E6A-471A-BCB4-2977DBFE912C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Produto</t>
   </si>
   <si>
-    <t>Categoria</t>
-  </si>
-  <si>
     <t>Marca</t>
   </si>
   <si>
@@ -337,6 +334,9 @@
   </si>
   <si>
     <t>350.00</t>
+  </si>
+  <si>
+    <t>Tipo do Produto</t>
   </si>
   <si>
     <t>Observação</t>
@@ -350,7 +350,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -453,22 +453,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,7 +749,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,540 +757,540 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="13"/>
+        <v>90</v>
+      </c>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="14"/>
+        <v>74</v>
+      </c>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="13"/>
+        <v>93</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="14"/>
+        <v>92</v>
+      </c>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="13"/>
+        <v>85</v>
+      </c>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" s="14"/>
+        <v>94</v>
+      </c>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="13"/>
+        <v>88</v>
+      </c>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="E11" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="14"/>
+        <v>95</v>
+      </c>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="13"/>
+        <v>81</v>
+      </c>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="14"/>
+        <v>96</v>
+      </c>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="13"/>
+        <v>82</v>
+      </c>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" s="14"/>
+        <v>97</v>
+      </c>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="13"/>
+        <v>98</v>
+      </c>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="14"/>
+        <v>82</v>
+      </c>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="13"/>
+        <v>99</v>
+      </c>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G19" s="14"/>
+        <v>100</v>
+      </c>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G21" s="14"/>
+        <v>100</v>
+      </c>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="13"/>
+        <v>75</v>
+      </c>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G23" s="14"/>
+        <v>101</v>
+      </c>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="13"/>
+        <v>97</v>
+      </c>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="14"/>
+        <v>95</v>
+      </c>
+      <c r="G25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>